<commit_message>
Selenium Element from lap
</commit_message>
<xml_diff>
--- a/Guru99_Banking_Project/src/main/java/com/gurubanking/testdata/TestData.xlsx
+++ b/Guru99_Banking_Project/src/main/java/com/gurubanking/testdata/TestData.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{383693B4-D5D0-45AD-A690-CF296ACFF53D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12615" windowHeight="2445" xr2:uid="{F6302E56-5DAE-4799-BD53-CC9FB1311A2B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13050" windowHeight="3330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H6"/>
+  <oleSize ref="A1:J9"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -138,7 +137,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -502,7 +501,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57774F33-E44B-4C6C-9D2D-978028B5ED8F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -588,14 +587,14 @@
     <row r="5" spans="1:10" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{3BD74228-201C-4E9B-878E-AF7E65298BCA}"/>
+    <hyperlink ref="I2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85902269-3405-4A9F-B57E-4B0EEB745CF9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>